<commit_message>
VPN Network Ticket Sample
</commit_message>
<xml_diff>
--- a/network_tickets/auto_tickets/VPN_Account_Ticket_Sample.xlsx
+++ b/network_tickets/auto_tickets/VPN_Account_Ticket_Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P7869\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9D4AA0-A7E1-4A1D-B10D-6D1AAC8D538A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006E6833-4E69-49A7-B59F-D3FF4CDE7FB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ticket No.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -50,28 +46,39 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>申请人工号（默认作为合作伙伴上级）</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>p1111</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leo</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test@test.com</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>合作伙伴邮箱(VPN的username，pwd请查收邮件)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>Phone Number</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>小李</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tes11t@test.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>测试</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8526847</t>
     </r>
     <r>
       <rPr>
@@ -80,58 +87,25 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>1</t>
+      <t>1234</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>测试</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test1@test.com</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test2@test.com</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phone Number</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>合作伙伴手机号码（默认+86）</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>测试</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test3@test.com</t>
+    <t>example</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test@hk.chinamobile.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>合作伙伴手机号码（默认+86）
+香港手机请加“+852”</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMHK申请人邮箱（默认作为合作伙伴上级）</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -142,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[DBNum2][$-804]General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -182,13 +156,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF7030A0"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="宋体"/>
@@ -204,15 +171,17 @@
       <name val="宋体"/>
     </font>
     <font>
-      <sz val="7"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -259,16 +228,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -282,30 +252,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="3" xr:uid="{8B951E07-CEF2-4091-A02E-574BC5C76B80}"/>
     <cellStyle name="常规 3" xfId="4" xr:uid="{F0979730-2B0F-464C-BCC4-9FAFA9E138C2}"/>
     <cellStyle name="常规 3 3" xfId="2" xr:uid="{19E02161-2882-45CB-8F26-19FE9CD30D8B}"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 8" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
@@ -583,15 +550,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.26953125" style="1" customWidth="1"/>
@@ -601,128 +568,64 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26">
       <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="54.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="14.5">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="13">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="10">
-        <v>13104259981</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.5">
-      <c r="A4" s="9">
-        <v>111</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="10">
-        <v>13104259982</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.5">
-      <c r="A5" s="9">
-        <v>111</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="10">
-        <v>13104259983</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.5">
-      <c r="A6" s="9">
-        <v>111</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10">
-        <v>13104259984</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.5">
-      <c r="A7" s="9">
-        <v>111</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="10">
-        <v>13104259984</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{A87332A2-46DA-4917-9542-B7B3B0AD8864}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8EDD58E4-5F05-44B0-A989-ECFE5AB88F2A}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;8&amp;F -- &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;8&amp;D  &amp;T&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>

</xml_diff>